<commit_message>
reading all file formats, needs big refactor
</commit_message>
<xml_diff>
--- a/Leerplanillacupos/data/data2024.1/030323.xlsx
+++ b/Leerplanillacupos/data/data2024.1/030323.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gastonmousques/workspace/ExcelExporter/excelconverter/Leerplanillacupos/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gastonmousques/workspace/IngSoftTools/excelconverter/Leerplanillacupos/data/data2024.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7ED3858-F36D-D54C-B1D4-DDBBBF052EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EB253C-8903-F040-9123-F5FEBD2BC3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="760" windowWidth="30160" windowHeight="18880" xr2:uid="{E2EAB03B-CC58-F343-82B4-968B67AFF3DB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="701">
   <si>
     <t>Id</t>
   </si>
@@ -2133,9 +2133,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Calidad de software</t>
-  </si>
-  <si>
-    <t>fecha</t>
   </si>
   <si>
     <t>Ins_Cupo</t>
@@ -2572,21 +2569,18 @@
   <dimension ref="A1:H302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="3" max="3" width="27.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.19921875" customWidth="1"/>
-    <col min="7" max="7" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>700</v>
-      </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2604,13 +2598,11 @@
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A2" s="9"/>
       <c r="B2" s="6">
         <v>64137</v>
       </c>
@@ -2632,9 +2624,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A3" s="9"/>
       <c r="B3" s="6">
         <v>64141</v>
       </c>
@@ -2658,9 +2648,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A4" s="9"/>
       <c r="B4" s="6">
         <v>64171</v>
       </c>
@@ -2684,9 +2672,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A5" s="9"/>
       <c r="B5" s="6">
         <v>64609</v>
       </c>
@@ -2710,9 +2696,7 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A6" s="9"/>
       <c r="B6" s="6">
         <v>64610</v>
       </c>
@@ -2736,9 +2720,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A7" s="9"/>
       <c r="B7" s="6">
         <v>64611</v>
       </c>
@@ -2762,9 +2744,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A8" s="9"/>
       <c r="B8" s="6">
         <v>64612</v>
       </c>
@@ -2788,9 +2768,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A9" s="9"/>
       <c r="B9" s="6">
         <v>65510</v>
       </c>
@@ -2814,9 +2792,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A10" s="9"/>
       <c r="B10" s="6">
         <v>65555</v>
       </c>
@@ -2840,9 +2816,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A11" s="9"/>
       <c r="B11" s="6">
         <v>64806</v>
       </c>
@@ -2866,9 +2840,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A12" s="9"/>
       <c r="B12" s="6">
         <v>65134</v>
       </c>
@@ -2892,9 +2864,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A13" s="9"/>
       <c r="B13" s="6">
         <v>64201</v>
       </c>
@@ -2918,9 +2888,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A14" s="9"/>
       <c r="B14" s="6">
         <v>64205</v>
       </c>
@@ -2944,9 +2912,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A15" s="9"/>
       <c r="B15" s="6">
         <v>64209</v>
       </c>
@@ -2970,9 +2936,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A16" s="9"/>
       <c r="B16" s="6">
         <v>64213</v>
       </c>
@@ -2996,9 +2960,7 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A17" s="9"/>
       <c r="B17" s="6">
         <v>64217</v>
       </c>
@@ -3022,9 +2984,7 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A18" s="9"/>
       <c r="B18" s="6">
         <v>64221</v>
       </c>
@@ -3048,9 +3008,7 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A19" s="9"/>
       <c r="B19" s="6">
         <v>64226</v>
       </c>
@@ -3074,9 +3032,7 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A20" s="9"/>
       <c r="B20" s="6">
         <v>64230</v>
       </c>
@@ -3100,9 +3056,7 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A21" s="9"/>
       <c r="B21" s="6">
         <v>64235</v>
       </c>
@@ -3126,9 +3080,7 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A22" s="9"/>
       <c r="B22" s="6">
         <v>64306</v>
       </c>
@@ -3152,9 +3104,7 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A23" s="9"/>
       <c r="B23" s="6">
         <v>64455</v>
       </c>
@@ -3178,9 +3128,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A24" s="9"/>
       <c r="B24" s="6">
         <v>64754</v>
       </c>
@@ -3202,9 +3150,7 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A25" s="9"/>
       <c r="B25" s="6">
         <v>64166</v>
       </c>
@@ -3228,9 +3174,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A26" s="9"/>
       <c r="B26" s="6">
         <v>64186</v>
       </c>
@@ -3254,9 +3198,7 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A27" s="9"/>
       <c r="B27" s="6">
         <v>64804</v>
       </c>
@@ -3280,9 +3222,7 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A28" s="9"/>
       <c r="B28" s="6">
         <v>64337</v>
       </c>
@@ -3306,9 +3246,7 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A29" s="9"/>
       <c r="B29" s="6">
         <v>65188</v>
       </c>
@@ -3332,9 +3270,7 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A30" s="9"/>
       <c r="B30" s="6">
         <v>64252</v>
       </c>
@@ -3358,9 +3294,7 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A31" s="9"/>
       <c r="B31" s="6">
         <v>64256</v>
       </c>
@@ -3384,9 +3318,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A32" s="9"/>
       <c r="B32" s="6">
         <v>64260</v>
       </c>
@@ -3410,9 +3342,7 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A33" s="9"/>
       <c r="B33" s="6">
         <v>64264</v>
       </c>
@@ -3436,9 +3366,7 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A34" s="9"/>
       <c r="B34" s="6">
         <v>64313</v>
       </c>
@@ -3462,9 +3390,7 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A35" s="9"/>
       <c r="B35" s="6">
         <v>64292</v>
       </c>
@@ -3488,9 +3414,7 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A36" s="9"/>
       <c r="B36" s="6">
         <v>64328</v>
       </c>
@@ -3514,9 +3438,7 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A37" s="9"/>
       <c r="B37" s="6">
         <v>64332</v>
       </c>
@@ -3540,9 +3462,7 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A38" s="9"/>
       <c r="B38" s="6">
         <v>64194</v>
       </c>
@@ -3566,9 +3486,7 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A39" s="9"/>
       <c r="B39" s="6">
         <v>65150</v>
       </c>
@@ -3592,9 +3510,7 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A40" s="9"/>
       <c r="B40" s="6">
         <v>64301</v>
       </c>
@@ -3618,9 +3534,7 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A41" s="9"/>
       <c r="B41" s="6">
         <v>64331</v>
       </c>
@@ -3644,9 +3558,7 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A42" s="9"/>
       <c r="B42" s="6">
         <v>64336</v>
       </c>
@@ -3670,9 +3582,7 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A43" s="9"/>
       <c r="B43" s="6">
         <v>64149</v>
       </c>
@@ -3696,9 +3606,7 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A44" s="9"/>
       <c r="B44" s="6">
         <v>64153</v>
       </c>
@@ -3722,9 +3630,7 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A45" s="9"/>
       <c r="B45" s="6">
         <v>64176</v>
       </c>
@@ -3748,9 +3654,7 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A46" s="9"/>
       <c r="B46" s="6">
         <v>64268</v>
       </c>
@@ -3774,9 +3678,7 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A47" s="9"/>
       <c r="B47" s="6">
         <v>64272</v>
       </c>
@@ -3800,9 +3702,7 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A48" s="9"/>
       <c r="B48" s="6">
         <v>64317</v>
       </c>
@@ -3826,9 +3726,7 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A49" s="9"/>
       <c r="B49" s="6">
         <v>64180</v>
       </c>
@@ -3852,9 +3750,7 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A50" s="9"/>
       <c r="B50" s="6">
         <v>64275</v>
       </c>
@@ -3878,9 +3774,7 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A51" s="9"/>
       <c r="B51" s="6">
         <v>64280</v>
       </c>
@@ -3904,9 +3798,7 @@
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A52" s="9"/>
       <c r="B52" s="6">
         <v>64285</v>
       </c>
@@ -3930,9 +3822,7 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A53" s="9"/>
       <c r="B53" s="6">
         <v>64319</v>
       </c>
@@ -3956,9 +3846,7 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A54" s="9"/>
       <c r="B54" s="6">
         <v>64188</v>
       </c>
@@ -3982,9 +3870,7 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A55" s="9"/>
       <c r="B55" s="6">
         <v>64813</v>
       </c>
@@ -4008,9 +3894,7 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A56" s="9"/>
       <c r="B56" s="6">
         <v>65257</v>
       </c>
@@ -4034,9 +3918,7 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A57" s="9"/>
       <c r="B57" s="6">
         <v>65309</v>
       </c>
@@ -4060,9 +3942,7 @@
       </c>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A58" s="9"/>
       <c r="B58" s="6">
         <v>65585</v>
       </c>
@@ -4086,9 +3966,7 @@
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A59" s="9"/>
       <c r="B59" s="6">
         <v>65586</v>
       </c>
@@ -4112,9 +3990,7 @@
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A60" s="9"/>
       <c r="B60" s="6">
         <v>65291</v>
       </c>
@@ -4138,9 +4014,7 @@
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A61" s="9"/>
       <c r="B61" s="6">
         <v>65406</v>
       </c>
@@ -4164,9 +4038,7 @@
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A62" s="9"/>
       <c r="B62" s="6">
         <v>65241</v>
       </c>
@@ -4190,9 +4062,7 @@
       </c>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A63" s="9"/>
       <c r="B63" s="6">
         <v>65293</v>
       </c>
@@ -4216,9 +4086,7 @@
       </c>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A64" s="9"/>
       <c r="B64" s="6">
         <v>65408</v>
       </c>
@@ -4242,9 +4110,7 @@
       </c>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A65" s="9"/>
       <c r="B65" s="6">
         <v>65253</v>
       </c>
@@ -4268,9 +4134,7 @@
       </c>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A66" s="9"/>
       <c r="B66" s="6">
         <v>64202</v>
       </c>
@@ -4292,9 +4156,7 @@
       </c>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A67" s="9"/>
       <c r="B67" s="6">
         <v>64206</v>
       </c>
@@ -4316,9 +4178,7 @@
       </c>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A68" s="9"/>
       <c r="B68" s="6">
         <v>64210</v>
       </c>
@@ -4342,9 +4202,7 @@
       </c>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A69" s="9"/>
       <c r="B69" s="6">
         <v>64214</v>
       </c>
@@ -4368,9 +4226,7 @@
       </c>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A70" s="9"/>
       <c r="B70" s="6">
         <v>64218</v>
       </c>
@@ -4394,9 +4250,7 @@
       </c>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A71" s="9"/>
       <c r="B71" s="6">
         <v>64222</v>
       </c>
@@ -4420,9 +4274,7 @@
       </c>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A72" s="9"/>
       <c r="B72" s="6">
         <v>64227</v>
       </c>
@@ -4444,9 +4296,7 @@
       </c>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A73" s="9"/>
       <c r="B73" s="6">
         <v>64231</v>
       </c>
@@ -4468,9 +4318,7 @@
       </c>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A74" s="9"/>
       <c r="B74" s="6">
         <v>64236</v>
       </c>
@@ -4494,9 +4342,7 @@
       </c>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A75" s="9"/>
       <c r="B75" s="6">
         <v>64307</v>
       </c>
@@ -4520,9 +4366,7 @@
       </c>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A76" s="9"/>
       <c r="B76" s="6">
         <v>64456</v>
       </c>
@@ -4546,9 +4390,7 @@
       </c>
     </row>
     <row r="77" spans="1:8">
-      <c r="A77" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A77" s="9"/>
       <c r="B77" s="6">
         <v>64460</v>
       </c>
@@ -4572,9 +4414,7 @@
       </c>
     </row>
     <row r="78" spans="1:8">
-      <c r="A78" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A78" s="9"/>
       <c r="B78" s="6">
         <v>65726</v>
       </c>
@@ -4598,9 +4438,7 @@
       </c>
     </row>
     <row r="79" spans="1:8">
-      <c r="A79" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A79" s="9"/>
       <c r="B79" s="6">
         <v>64459</v>
       </c>
@@ -4624,9 +4462,7 @@
       </c>
     </row>
     <row r="80" spans="1:8">
-      <c r="A80" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A80" s="9"/>
       <c r="B80" s="6">
         <v>64303</v>
       </c>
@@ -4650,9 +4486,7 @@
       </c>
     </row>
     <row r="81" spans="1:8">
-      <c r="A81" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A81" s="9"/>
       <c r="B81" s="6">
         <v>64335</v>
       </c>
@@ -4676,9 +4510,7 @@
       </c>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A82" s="9"/>
       <c r="B82" s="6">
         <v>64812</v>
       </c>
@@ -4702,9 +4534,7 @@
       </c>
     </row>
     <row r="83" spans="1:8">
-      <c r="A83" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A83" s="9"/>
       <c r="B83" s="6">
         <v>64195</v>
       </c>
@@ -4728,9 +4558,7 @@
       </c>
     </row>
     <row r="84" spans="1:8">
-      <c r="A84" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A84" s="9"/>
       <c r="B84" s="6">
         <v>64856</v>
       </c>
@@ -4754,9 +4582,7 @@
       </c>
     </row>
     <row r="85" spans="1:8">
-      <c r="A85" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A85" s="9"/>
       <c r="B85" s="6">
         <v>65541</v>
       </c>
@@ -4780,9 +4606,7 @@
       </c>
     </row>
     <row r="86" spans="1:8">
-      <c r="A86" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A86" s="9"/>
       <c r="B86" s="6">
         <v>65153</v>
       </c>
@@ -4806,9 +4630,7 @@
       </c>
     </row>
     <row r="87" spans="1:8">
-      <c r="A87" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A87" s="9"/>
       <c r="B87" s="6">
         <v>64159</v>
       </c>
@@ -4832,9 +4654,7 @@
       </c>
     </row>
     <row r="88" spans="1:8">
-      <c r="A88" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A88" s="9"/>
       <c r="B88" s="6">
         <v>64179</v>
       </c>
@@ -4858,9 +4678,7 @@
       </c>
     </row>
     <row r="89" spans="1:8">
-      <c r="A89" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A89" s="9"/>
       <c r="B89" s="6">
         <v>64274</v>
       </c>
@@ -4884,9 +4702,7 @@
       </c>
     </row>
     <row r="90" spans="1:8">
-      <c r="A90" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A90" s="9"/>
       <c r="B90" s="6">
         <v>64279</v>
       </c>
@@ -4910,9 +4726,7 @@
       </c>
     </row>
     <row r="91" spans="1:8">
-      <c r="A91" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A91" s="9"/>
       <c r="B91" s="6">
         <v>64284</v>
       </c>
@@ -4936,9 +4750,7 @@
       </c>
     </row>
     <row r="92" spans="1:8">
-      <c r="A92" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A92" s="9"/>
       <c r="B92" s="6">
         <v>64318</v>
       </c>
@@ -4962,9 +4774,7 @@
       </c>
     </row>
     <row r="93" spans="1:8">
-      <c r="A93" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A93" s="9"/>
       <c r="B93" s="6">
         <v>64163</v>
       </c>
@@ -4988,9 +4798,7 @@
       </c>
     </row>
     <row r="94" spans="1:8">
-      <c r="A94" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A94" s="9"/>
       <c r="B94" s="6">
         <v>64183</v>
       </c>
@@ -5014,9 +4822,7 @@
       </c>
     </row>
     <row r="95" spans="1:8">
-      <c r="A95" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A95" s="9"/>
       <c r="B95" s="6">
         <v>64289</v>
       </c>
@@ -5040,9 +4846,7 @@
       </c>
     </row>
     <row r="96" spans="1:8">
-      <c r="A96" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A96" s="9"/>
       <c r="B96" s="6">
         <v>64323</v>
       </c>
@@ -5066,9 +4870,7 @@
       </c>
     </row>
     <row r="97" spans="1:8">
-      <c r="A97" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A97" s="9"/>
       <c r="B97" s="6">
         <v>64486</v>
       </c>
@@ -5092,9 +4894,7 @@
       </c>
     </row>
     <row r="98" spans="1:8">
-      <c r="A98" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A98" s="9"/>
       <c r="B98" s="6">
         <v>64489</v>
       </c>
@@ -5118,9 +4918,7 @@
       </c>
     </row>
     <row r="99" spans="1:8">
-      <c r="A99" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A99" s="9"/>
       <c r="B99" s="6">
         <v>64490</v>
       </c>
@@ -5144,9 +4942,7 @@
       </c>
     </row>
     <row r="100" spans="1:8">
-      <c r="A100" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A100" s="9"/>
       <c r="B100" s="6">
         <v>65156</v>
       </c>
@@ -5170,9 +4966,7 @@
       </c>
     </row>
     <row r="101" spans="1:8">
-      <c r="A101" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A101" s="9"/>
       <c r="B101" s="6">
         <v>64774</v>
       </c>
@@ -5196,9 +4990,7 @@
       </c>
     </row>
     <row r="102" spans="1:8">
-      <c r="A102" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A102" s="9"/>
       <c r="B102" s="6">
         <v>64197</v>
       </c>
@@ -5222,9 +5014,7 @@
       </c>
     </row>
     <row r="103" spans="1:8">
-      <c r="A103" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A103" s="9"/>
       <c r="B103" s="6">
         <v>64148</v>
       </c>
@@ -5248,9 +5038,7 @@
       </c>
     </row>
     <row r="104" spans="1:8">
-      <c r="A104" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A104" s="9"/>
       <c r="B104" s="6">
         <v>64152</v>
       </c>
@@ -5274,9 +5062,7 @@
       </c>
     </row>
     <row r="105" spans="1:8">
-      <c r="A105" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A105" s="9"/>
       <c r="B105" s="6">
         <v>64175</v>
       </c>
@@ -5300,9 +5086,7 @@
       </c>
     </row>
     <row r="106" spans="1:8">
-      <c r="A106" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A106" s="9"/>
       <c r="B106" s="6">
         <v>64249</v>
       </c>
@@ -5326,9 +5110,7 @@
       </c>
     </row>
     <row r="107" spans="1:8">
-      <c r="A107" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A107" s="9"/>
       <c r="B107" s="6">
         <v>64253</v>
       </c>
@@ -5352,9 +5134,7 @@
       </c>
     </row>
     <row r="108" spans="1:8">
-      <c r="A108" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A108" s="9"/>
       <c r="B108" s="6">
         <v>64257</v>
       </c>
@@ -5378,9 +5158,7 @@
       </c>
     </row>
     <row r="109" spans="1:8">
-      <c r="A109" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A109" s="9"/>
       <c r="B109" s="6">
         <v>64261</v>
       </c>
@@ -5404,9 +5182,7 @@
       </c>
     </row>
     <row r="110" spans="1:8">
-      <c r="A110" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A110" s="9"/>
       <c r="B110" s="6">
         <v>64310</v>
       </c>
@@ -5430,9 +5206,7 @@
       </c>
     </row>
     <row r="111" spans="1:8">
-      <c r="A111" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A111" s="9"/>
       <c r="B111" s="6">
         <v>64458</v>
       </c>
@@ -5456,9 +5230,7 @@
       </c>
     </row>
     <row r="112" spans="1:8">
-      <c r="A112" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A112" s="9"/>
       <c r="B112" s="6">
         <v>64265</v>
       </c>
@@ -5482,9 +5254,7 @@
       </c>
     </row>
     <row r="113" spans="1:8">
-      <c r="A113" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A113" s="9"/>
       <c r="B113" s="6">
         <v>64270</v>
       </c>
@@ -5508,9 +5278,7 @@
       </c>
     </row>
     <row r="114" spans="1:8">
-      <c r="A114" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A114" s="9"/>
       <c r="B114" s="6">
         <v>64314</v>
       </c>
@@ -5534,9 +5302,7 @@
       </c>
     </row>
     <row r="115" spans="1:8">
-      <c r="A115" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A115" s="9"/>
       <c r="B115" s="6">
         <v>65273</v>
       </c>
@@ -5560,9 +5326,7 @@
       </c>
     </row>
     <row r="116" spans="1:8">
-      <c r="A116" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A116" s="9"/>
       <c r="B116" s="6">
         <v>64192</v>
       </c>
@@ -5586,9 +5350,7 @@
       </c>
     </row>
     <row r="117" spans="1:8">
-      <c r="A117" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A117" s="9"/>
       <c r="B117" s="6">
         <v>64880</v>
       </c>
@@ -5612,9 +5374,7 @@
       </c>
     </row>
     <row r="118" spans="1:8">
-      <c r="A118" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A118" s="9"/>
       <c r="B118" s="6">
         <v>64461</v>
       </c>
@@ -5638,9 +5398,7 @@
       </c>
     </row>
     <row r="119" spans="1:8">
-      <c r="A119" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A119" s="9"/>
       <c r="B119" s="6">
         <v>65294</v>
       </c>
@@ -5664,9 +5422,7 @@
       </c>
     </row>
     <row r="120" spans="1:8">
-      <c r="A120" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A120" s="9"/>
       <c r="B120" s="6">
         <v>65409</v>
       </c>
@@ -5690,9 +5446,7 @@
       </c>
     </row>
     <row r="121" spans="1:8">
-      <c r="A121" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A121" s="9"/>
       <c r="B121" s="6">
         <v>65292</v>
       </c>
@@ -5716,9 +5470,7 @@
       </c>
     </row>
     <row r="122" spans="1:8">
-      <c r="A122" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A122" s="9"/>
       <c r="B122" s="6">
         <v>65407</v>
       </c>
@@ -5742,9 +5494,7 @@
       </c>
     </row>
     <row r="123" spans="1:8">
-      <c r="A123" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A123" s="9"/>
       <c r="B123" s="6">
         <v>64240</v>
       </c>
@@ -5768,9 +5518,7 @@
       </c>
     </row>
     <row r="124" spans="1:8">
-      <c r="A124" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A124" s="9"/>
       <c r="B124" s="6">
         <v>64244</v>
       </c>
@@ -5794,9 +5542,7 @@
       </c>
     </row>
     <row r="125" spans="1:8">
-      <c r="A125" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A125" s="9"/>
       <c r="B125" s="6">
         <v>64785</v>
       </c>
@@ -5820,9 +5566,7 @@
       </c>
     </row>
     <row r="126" spans="1:8">
-      <c r="A126" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A126" s="9"/>
       <c r="B126" s="6">
         <v>64238</v>
       </c>
@@ -5846,9 +5590,7 @@
       </c>
     </row>
     <row r="127" spans="1:8">
-      <c r="A127" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A127" s="9"/>
       <c r="B127" s="6">
         <v>64242</v>
       </c>
@@ -5872,9 +5614,7 @@
       </c>
     </row>
     <row r="128" spans="1:8">
-      <c r="A128" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A128" s="9"/>
       <c r="B128" s="6">
         <v>64309</v>
       </c>
@@ -5898,9 +5638,7 @@
       </c>
     </row>
     <row r="129" spans="1:8">
-      <c r="A129" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A129" s="9"/>
       <c r="B129" s="6">
         <v>64154</v>
       </c>
@@ -5924,9 +5662,7 @@
       </c>
     </row>
     <row r="130" spans="1:8">
-      <c r="A130" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A130" s="9"/>
       <c r="B130" s="6">
         <v>64177</v>
       </c>
@@ -5950,9 +5686,7 @@
       </c>
     </row>
     <row r="131" spans="1:8">
-      <c r="A131" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A131" s="9"/>
       <c r="B131" s="6">
         <v>64269</v>
       </c>
@@ -5976,9 +5710,7 @@
       </c>
     </row>
     <row r="132" spans="1:8">
-      <c r="A132" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A132" s="9"/>
       <c r="B132" s="6">
         <v>64273</v>
       </c>
@@ -6002,9 +5734,7 @@
       </c>
     </row>
     <row r="133" spans="1:8">
-      <c r="A133" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A133" s="9"/>
       <c r="B133" s="6">
         <v>64315</v>
       </c>
@@ -6028,9 +5758,7 @@
       </c>
     </row>
     <row r="134" spans="1:8">
-      <c r="A134" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A134" s="9"/>
       <c r="B134" s="6">
         <v>64136</v>
       </c>
@@ -6052,9 +5780,7 @@
       </c>
     </row>
     <row r="135" spans="1:8">
-      <c r="A135" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A135" s="9"/>
       <c r="B135" s="6">
         <v>64140</v>
       </c>
@@ -6078,9 +5804,7 @@
       </c>
     </row>
     <row r="136" spans="1:8">
-      <c r="A136" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A136" s="9"/>
       <c r="B136" s="6">
         <v>64170</v>
       </c>
@@ -6104,9 +5828,7 @@
       </c>
     </row>
     <row r="137" spans="1:8">
-      <c r="A137" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A137" s="9"/>
       <c r="B137" s="6">
         <v>65546</v>
       </c>
@@ -6130,9 +5852,7 @@
       </c>
     </row>
     <row r="138" spans="1:8">
-      <c r="A138" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A138" s="9"/>
       <c r="B138" s="6">
         <v>65547</v>
       </c>
@@ -6156,9 +5876,7 @@
       </c>
     </row>
     <row r="139" spans="1:8">
-      <c r="A139" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A139" s="9"/>
       <c r="B139" s="6">
         <v>64144</v>
       </c>
@@ -6182,9 +5900,7 @@
       </c>
     </row>
     <row r="140" spans="1:8">
-      <c r="A140" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A140" s="9"/>
       <c r="B140" s="6">
         <v>64147</v>
       </c>
@@ -6208,9 +5924,7 @@
       </c>
     </row>
     <row r="141" spans="1:8">
-      <c r="A141" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A141" s="9"/>
       <c r="B141" s="6">
         <v>64174</v>
       </c>
@@ -6234,9 +5948,7 @@
       </c>
     </row>
     <row r="142" spans="1:8">
-      <c r="A142" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A142" s="9"/>
       <c r="B142" s="6">
         <v>65254</v>
       </c>
@@ -6260,9 +5972,7 @@
       </c>
     </row>
     <row r="143" spans="1:8">
-      <c r="A143" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A143" s="9"/>
       <c r="B143" s="6">
         <v>64814</v>
       </c>
@@ -6286,9 +5996,7 @@
       </c>
     </row>
     <row r="144" spans="1:8">
-      <c r="A144" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A144" s="9"/>
       <c r="B144" s="6">
         <v>64815</v>
       </c>
@@ -6312,9 +6020,7 @@
       </c>
     </row>
     <row r="145" spans="1:8">
-      <c r="A145" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A145" s="9"/>
       <c r="B145" s="6">
         <v>64196</v>
       </c>
@@ -6338,9 +6044,7 @@
       </c>
     </row>
     <row r="146" spans="1:8">
-      <c r="A146" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A146" s="9"/>
       <c r="B146" s="6">
         <v>64291</v>
       </c>
@@ -6364,9 +6068,7 @@
       </c>
     </row>
     <row r="147" spans="1:8">
-      <c r="A147" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A147" s="9"/>
       <c r="B147" s="6">
         <v>64162</v>
       </c>
@@ -6390,9 +6092,7 @@
       </c>
     </row>
     <row r="148" spans="1:8">
-      <c r="A148" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A148" s="9"/>
       <c r="B148" s="6">
         <v>64182</v>
       </c>
@@ -6416,9 +6116,7 @@
       </c>
     </row>
     <row r="149" spans="1:8">
-      <c r="A149" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A149" s="9"/>
       <c r="B149" s="6">
         <v>65157</v>
       </c>
@@ -6442,9 +6140,7 @@
       </c>
     </row>
     <row r="150" spans="1:8">
-      <c r="A150" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A150" s="9"/>
       <c r="B150" s="6">
         <v>64191</v>
       </c>
@@ -6468,9 +6164,7 @@
       </c>
     </row>
     <row r="151" spans="1:8">
-      <c r="A151" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A151" s="9"/>
       <c r="B151" s="6">
         <v>64290</v>
       </c>
@@ -6494,9 +6188,7 @@
       </c>
     </row>
     <row r="152" spans="1:8">
-      <c r="A152" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A152" s="9"/>
       <c r="B152" s="6">
         <v>64325</v>
       </c>
@@ -6520,9 +6212,7 @@
       </c>
     </row>
     <row r="153" spans="1:8">
-      <c r="A153" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A153" s="9"/>
       <c r="B153" s="6">
         <v>64300</v>
       </c>
@@ -6546,9 +6236,7 @@
       </c>
     </row>
     <row r="154" spans="1:8">
-      <c r="A154" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A154" s="9"/>
       <c r="B154" s="6">
         <v>64329</v>
       </c>
@@ -6572,9 +6260,7 @@
       </c>
     </row>
     <row r="155" spans="1:8">
-      <c r="A155" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A155" s="9"/>
       <c r="B155" s="6">
         <v>64333</v>
       </c>
@@ -6598,9 +6284,7 @@
       </c>
     </row>
     <row r="156" spans="1:8">
-      <c r="A156" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A156" s="9"/>
       <c r="B156" s="6">
         <v>65278</v>
       </c>
@@ -6624,9 +6308,7 @@
       </c>
     </row>
     <row r="157" spans="1:8">
-      <c r="A157" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A157" s="9"/>
       <c r="B157" s="6">
         <v>64457</v>
       </c>
@@ -6650,9 +6332,7 @@
       </c>
     </row>
     <row r="158" spans="1:8">
-      <c r="A158" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A158" s="9"/>
       <c r="B158" s="6">
         <v>64487</v>
       </c>
@@ -6676,9 +6356,7 @@
       </c>
     </row>
     <row r="159" spans="1:8">
-      <c r="A159" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A159" s="9"/>
       <c r="B159" s="6">
         <v>64475</v>
       </c>
@@ -6702,9 +6380,7 @@
       </c>
     </row>
     <row r="160" spans="1:8">
-      <c r="A160" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A160" s="9"/>
       <c r="B160" s="6">
         <v>64302</v>
       </c>
@@ -6728,9 +6404,7 @@
       </c>
     </row>
     <row r="161" spans="1:8">
-      <c r="A161" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A161" s="9"/>
       <c r="B161" s="6">
         <v>64330</v>
       </c>
@@ -6754,9 +6428,7 @@
       </c>
     </row>
     <row r="162" spans="1:8">
-      <c r="A162" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A162" s="9"/>
       <c r="B162" s="6">
         <v>64334</v>
       </c>
@@ -6780,9 +6452,7 @@
       </c>
     </row>
     <row r="163" spans="1:8">
-      <c r="A163" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A163" s="9"/>
       <c r="B163" s="6">
         <v>64339</v>
       </c>
@@ -6806,9 +6476,7 @@
       </c>
     </row>
     <row r="164" spans="1:8">
-      <c r="A164" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A164" s="9"/>
       <c r="B164" s="6">
         <v>64799</v>
       </c>
@@ -6832,9 +6500,7 @@
       </c>
     </row>
     <row r="165" spans="1:8">
-      <c r="A165" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A165" s="9"/>
       <c r="B165" s="6">
         <v>65311</v>
       </c>
@@ -6858,9 +6524,7 @@
       </c>
     </row>
     <row r="166" spans="1:8">
-      <c r="A166" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A166" s="9"/>
       <c r="B166" s="6">
         <v>65587</v>
       </c>
@@ -6884,9 +6548,7 @@
       </c>
     </row>
     <row r="167" spans="1:8">
-      <c r="A167" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A167" s="9"/>
       <c r="B167" s="6">
         <v>65588</v>
       </c>
@@ -6910,9 +6572,7 @@
       </c>
     </row>
     <row r="168" spans="1:8">
-      <c r="A168" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A168" s="9"/>
       <c r="B168" s="6">
         <v>65317</v>
       </c>
@@ -6936,9 +6596,7 @@
       </c>
     </row>
     <row r="169" spans="1:8">
-      <c r="A169" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A169" s="9"/>
       <c r="B169" s="6">
         <v>65318</v>
       </c>
@@ -6962,9 +6620,7 @@
       </c>
     </row>
     <row r="170" spans="1:8">
-      <c r="A170" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A170" s="9"/>
       <c r="B170" s="6">
         <v>65319</v>
       </c>
@@ -6988,9 +6644,7 @@
       </c>
     </row>
     <row r="171" spans="1:8">
-      <c r="A171" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A171" s="9"/>
       <c r="B171" s="6">
         <v>65320</v>
       </c>
@@ -7014,9 +6668,7 @@
       </c>
     </row>
     <row r="172" spans="1:8">
-      <c r="A172" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A172" s="9"/>
       <c r="B172" s="6">
         <v>65321</v>
       </c>
@@ -7040,9 +6692,7 @@
       </c>
     </row>
     <row r="173" spans="1:8">
-      <c r="A173" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A173" s="9"/>
       <c r="B173" s="6">
         <v>65258</v>
       </c>
@@ -7066,9 +6716,7 @@
       </c>
     </row>
     <row r="174" spans="1:8">
-      <c r="A174" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A174" s="9"/>
       <c r="B174" s="6">
         <v>65279</v>
       </c>
@@ -7092,9 +6740,7 @@
       </c>
     </row>
     <row r="175" spans="1:8">
-      <c r="A175" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A175" s="9"/>
       <c r="B175" s="6">
         <v>65280</v>
       </c>
@@ -7118,9 +6764,7 @@
       </c>
     </row>
     <row r="176" spans="1:8">
-      <c r="A176" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A176" s="9"/>
       <c r="B176" s="6">
         <v>65281</v>
       </c>
@@ -7144,9 +6788,7 @@
       </c>
     </row>
     <row r="177" spans="1:8">
-      <c r="A177" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A177" s="9"/>
       <c r="B177" s="6">
         <v>65282</v>
       </c>
@@ -7170,9 +6812,7 @@
       </c>
     </row>
     <row r="178" spans="1:8">
-      <c r="A178" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A178" s="9"/>
       <c r="B178" s="6">
         <v>65295</v>
       </c>
@@ -7196,9 +6836,7 @@
       </c>
     </row>
     <row r="179" spans="1:8">
-      <c r="A179" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A179" s="9"/>
       <c r="B179" s="6">
         <v>65296</v>
       </c>
@@ -7222,9 +6860,7 @@
       </c>
     </row>
     <row r="180" spans="1:8">
-      <c r="A180" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A180" s="9"/>
       <c r="B180" s="6">
         <v>65297</v>
       </c>
@@ -7248,9 +6884,7 @@
       </c>
     </row>
     <row r="181" spans="1:8">
-      <c r="A181" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A181" s="9"/>
       <c r="B181" s="6">
         <v>65298</v>
       </c>
@@ -7274,9 +6908,7 @@
       </c>
     </row>
     <row r="182" spans="1:8">
-      <c r="A182" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A182" s="9"/>
       <c r="B182" s="6">
         <v>64338</v>
       </c>
@@ -7300,9 +6932,7 @@
       </c>
     </row>
     <row r="183" spans="1:8">
-      <c r="A183" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A183" s="9"/>
       <c r="B183" s="6">
         <v>64250</v>
       </c>
@@ -7326,9 +6956,7 @@
       </c>
     </row>
     <row r="184" spans="1:8">
-      <c r="A184" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A184" s="9"/>
       <c r="B184" s="6">
         <v>64254</v>
       </c>
@@ -7352,9 +6980,7 @@
       </c>
     </row>
     <row r="185" spans="1:8">
-      <c r="A185" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A185" s="9"/>
       <c r="B185" s="6">
         <v>64258</v>
       </c>
@@ -7378,9 +7004,7 @@
       </c>
     </row>
     <row r="186" spans="1:8">
-      <c r="A186" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A186" s="9"/>
       <c r="B186" s="6">
         <v>64262</v>
       </c>
@@ -7404,9 +7028,7 @@
       </c>
     </row>
     <row r="187" spans="1:8">
-      <c r="A187" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A187" s="9"/>
       <c r="B187" s="6">
         <v>64311</v>
       </c>
@@ -7430,9 +7052,7 @@
       </c>
     </row>
     <row r="188" spans="1:8">
-      <c r="A188" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A188" s="9"/>
       <c r="B188" s="6">
         <v>64143</v>
       </c>
@@ -7456,9 +7076,7 @@
       </c>
     </row>
     <row r="189" spans="1:8">
-      <c r="A189" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A189" s="9"/>
       <c r="B189" s="6">
         <v>64146</v>
       </c>
@@ -7482,9 +7100,7 @@
       </c>
     </row>
     <row r="190" spans="1:8">
-      <c r="A190" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A190" s="9"/>
       <c r="B190" s="6">
         <v>64173</v>
       </c>
@@ -7508,9 +7124,7 @@
       </c>
     </row>
     <row r="191" spans="1:8">
-      <c r="A191" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A191" s="9"/>
       <c r="B191" s="6">
         <v>64190</v>
       </c>
@@ -7534,9 +7148,7 @@
       </c>
     </row>
     <row r="192" spans="1:8">
-      <c r="A192" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A192" s="9"/>
       <c r="B192" s="6">
         <v>64326</v>
       </c>
@@ -7560,9 +7172,7 @@
       </c>
     </row>
     <row r="193" spans="1:8">
-      <c r="A193" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A193" s="9"/>
       <c r="B193" s="6">
         <v>64757</v>
       </c>
@@ -7586,9 +7196,7 @@
       </c>
     </row>
     <row r="194" spans="1:8">
-      <c r="A194" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A194" s="9"/>
       <c r="B194" s="6">
         <v>64808</v>
       </c>
@@ -7610,9 +7218,7 @@
       </c>
     </row>
     <row r="195" spans="1:8">
-      <c r="A195" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A195" s="9"/>
       <c r="B195" s="6">
         <v>64488</v>
       </c>
@@ -7636,9 +7242,7 @@
       </c>
     </row>
     <row r="196" spans="1:8">
-      <c r="A196" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A196" s="9"/>
       <c r="B196" s="6">
         <v>64151</v>
       </c>
@@ -7662,9 +7266,7 @@
       </c>
     </row>
     <row r="197" spans="1:8">
-      <c r="A197" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A197" s="9"/>
       <c r="B197" s="6">
         <v>64155</v>
       </c>
@@ -7688,9 +7290,7 @@
       </c>
     </row>
     <row r="198" spans="1:8">
-      <c r="A198" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A198" s="9"/>
       <c r="B198" s="6">
         <v>64178</v>
       </c>
@@ -7714,9 +7314,7 @@
       </c>
     </row>
     <row r="199" spans="1:8">
-      <c r="A199" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A199" s="9"/>
       <c r="B199" s="6">
         <v>65314</v>
       </c>
@@ -7740,9 +7338,7 @@
       </c>
     </row>
     <row r="200" spans="1:8">
-      <c r="A200" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A200" s="9"/>
       <c r="B200" s="6">
         <v>65548</v>
       </c>
@@ -7764,9 +7360,7 @@
       </c>
     </row>
     <row r="201" spans="1:8">
-      <c r="A201" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A201" s="9"/>
       <c r="B201" s="6">
         <v>65549</v>
       </c>
@@ -7790,9 +7384,7 @@
       </c>
     </row>
     <row r="202" spans="1:8">
-      <c r="A202" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A202" s="9"/>
       <c r="B202" s="6">
         <v>64239</v>
       </c>
@@ -7816,9 +7408,7 @@
       </c>
     </row>
     <row r="203" spans="1:8">
-      <c r="A203" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A203" s="9"/>
       <c r="B203" s="6">
         <v>64243</v>
       </c>
@@ -7842,9 +7432,7 @@
       </c>
     </row>
     <row r="204" spans="1:8">
-      <c r="A204" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A204" s="9"/>
       <c r="B204" s="6">
         <v>65159</v>
       </c>
@@ -7868,9 +7456,7 @@
       </c>
     </row>
     <row r="205" spans="1:8">
-      <c r="A205" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A205" s="9"/>
       <c r="B205" s="6">
         <v>64164</v>
       </c>
@@ -7894,9 +7480,7 @@
       </c>
     </row>
     <row r="206" spans="1:8">
-      <c r="A206" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A206" s="9"/>
       <c r="B206" s="6">
         <v>64184</v>
       </c>
@@ -7920,9 +7504,7 @@
       </c>
     </row>
     <row r="207" spans="1:8">
-      <c r="A207" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A207" s="9"/>
       <c r="B207" s="6">
         <v>65276</v>
       </c>
@@ -7946,9 +7528,7 @@
       </c>
     </row>
     <row r="208" spans="1:8">
-      <c r="A208" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A208" s="9"/>
       <c r="B208" s="6">
         <v>65403</v>
       </c>
@@ -7972,9 +7552,7 @@
       </c>
     </row>
     <row r="209" spans="1:8">
-      <c r="A209" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A209" s="9"/>
       <c r="B209" s="6">
         <v>64816</v>
       </c>
@@ -7998,9 +7576,7 @@
       </c>
     </row>
     <row r="210" spans="1:8">
-      <c r="A210" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A210" s="9"/>
       <c r="B210" s="6">
         <v>64800</v>
       </c>
@@ -8024,9 +7600,7 @@
       </c>
     </row>
     <row r="211" spans="1:8">
-      <c r="A211" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A211" s="9"/>
       <c r="B211" s="6">
         <v>64476</v>
       </c>
@@ -8050,9 +7624,7 @@
       </c>
     </row>
     <row r="212" spans="1:8">
-      <c r="A212" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A212" s="9"/>
       <c r="B212" s="6">
         <v>64474</v>
       </c>
@@ -8076,9 +7648,7 @@
       </c>
     </row>
     <row r="213" spans="1:8">
-      <c r="A213" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A213" s="9"/>
       <c r="B213" s="6">
         <v>64267</v>
       </c>
@@ -8102,9 +7672,7 @@
       </c>
     </row>
     <row r="214" spans="1:8">
-      <c r="A214" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A214" s="9"/>
       <c r="B214" s="6">
         <v>64161</v>
       </c>
@@ -8128,9 +7696,7 @@
       </c>
     </row>
     <row r="215" spans="1:8">
-      <c r="A215" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A215" s="9"/>
       <c r="B215" s="6">
         <v>64181</v>
       </c>
@@ -8154,9 +7720,7 @@
       </c>
     </row>
     <row r="216" spans="1:8">
-      <c r="A216" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A216" s="9"/>
       <c r="B216" s="6">
         <v>64251</v>
       </c>
@@ -8180,9 +7744,7 @@
       </c>
     </row>
     <row r="217" spans="1:8">
-      <c r="A217" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A217" s="9"/>
       <c r="B217" s="6">
         <v>64255</v>
       </c>
@@ -8206,9 +7768,7 @@
       </c>
     </row>
     <row r="218" spans="1:8">
-      <c r="A218" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A218" s="9"/>
       <c r="B218" s="6">
         <v>64259</v>
       </c>
@@ -8232,9 +7792,7 @@
       </c>
     </row>
     <row r="219" spans="1:8">
-      <c r="A219" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A219" s="9"/>
       <c r="B219" s="6">
         <v>64263</v>
       </c>
@@ -8258,9 +7816,7 @@
       </c>
     </row>
     <row r="220" spans="1:8">
-      <c r="A220" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A220" s="9"/>
       <c r="B220" s="6">
         <v>64312</v>
       </c>
@@ -8284,9 +7840,7 @@
       </c>
     </row>
     <row r="221" spans="1:8">
-      <c r="A221" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A221" s="9"/>
       <c r="B221" s="6">
         <v>65290</v>
       </c>
@@ -8310,9 +7864,7 @@
       </c>
     </row>
     <row r="222" spans="1:8">
-      <c r="A222" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A222" s="9"/>
       <c r="B222" s="6">
         <v>65405</v>
       </c>
@@ -8336,9 +7888,7 @@
       </c>
     </row>
     <row r="223" spans="1:8">
-      <c r="A223" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A223" s="9"/>
       <c r="B223" s="6">
         <v>65277</v>
       </c>
@@ -8362,9 +7912,7 @@
       </c>
     </row>
     <row r="224" spans="1:8">
-      <c r="A224" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A224" s="9"/>
       <c r="B224" s="6">
         <v>65404</v>
       </c>
@@ -8388,9 +7936,7 @@
       </c>
     </row>
     <row r="225" spans="1:8">
-      <c r="A225" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A225" s="9"/>
       <c r="B225" s="6">
         <v>64134</v>
       </c>
@@ -8414,9 +7960,7 @@
       </c>
     </row>
     <row r="226" spans="1:8">
-      <c r="A226" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A226" s="9"/>
       <c r="B226" s="6">
         <v>64138</v>
       </c>
@@ -8440,9 +7984,7 @@
       </c>
     </row>
     <row r="227" spans="1:8">
-      <c r="A227" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A227" s="9"/>
       <c r="B227" s="6">
         <v>64168</v>
       </c>
@@ -8466,9 +8008,7 @@
       </c>
     </row>
     <row r="228" spans="1:8">
-      <c r="A228" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A228" s="9"/>
       <c r="B228" s="6">
         <v>64199</v>
       </c>
@@ -8492,9 +8032,7 @@
       </c>
     </row>
     <row r="229" spans="1:8">
-      <c r="A229" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A229" s="9"/>
       <c r="B229" s="6">
         <v>64203</v>
       </c>
@@ -8518,9 +8056,7 @@
       </c>
     </row>
     <row r="230" spans="1:8">
-      <c r="A230" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A230" s="9"/>
       <c r="B230" s="6">
         <v>64207</v>
       </c>
@@ -8544,9 +8080,7 @@
       </c>
     </row>
     <row r="231" spans="1:8">
-      <c r="A231" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A231" s="9"/>
       <c r="B231" s="6">
         <v>64211</v>
       </c>
@@ -8570,9 +8104,7 @@
       </c>
     </row>
     <row r="232" spans="1:8">
-      <c r="A232" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A232" s="9"/>
       <c r="B232" s="6">
         <v>64215</v>
       </c>
@@ -8596,9 +8128,7 @@
       </c>
     </row>
     <row r="233" spans="1:8">
-      <c r="A233" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A233" s="9"/>
       <c r="B233" s="6">
         <v>64219</v>
       </c>
@@ -8622,9 +8152,7 @@
       </c>
     </row>
     <row r="234" spans="1:8">
-      <c r="A234" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A234" s="9"/>
       <c r="B234" s="6">
         <v>64223</v>
       </c>
@@ -8648,9 +8176,7 @@
       </c>
     </row>
     <row r="235" spans="1:8">
-      <c r="A235" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A235" s="9"/>
       <c r="B235" s="6">
         <v>64228</v>
       </c>
@@ -8674,9 +8200,7 @@
       </c>
     </row>
     <row r="236" spans="1:8">
-      <c r="A236" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A236" s="9"/>
       <c r="B236" s="6">
         <v>64233</v>
       </c>
@@ -8700,9 +8224,7 @@
       </c>
     </row>
     <row r="237" spans="1:8">
-      <c r="A237" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A237" s="9"/>
       <c r="B237" s="6">
         <v>64304</v>
       </c>
@@ -8726,9 +8248,7 @@
       </c>
     </row>
     <row r="238" spans="1:8">
-      <c r="A238" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A238" s="9"/>
       <c r="B238" s="6">
         <v>65504</v>
       </c>
@@ -8750,9 +8270,7 @@
       </c>
     </row>
     <row r="239" spans="1:8">
-      <c r="A239" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A239" s="9"/>
       <c r="B239" s="6">
         <v>65508</v>
       </c>
@@ -8776,9 +8294,7 @@
       </c>
     </row>
     <row r="240" spans="1:8">
-      <c r="A240" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A240" s="9"/>
       <c r="B240" s="6">
         <v>64142</v>
       </c>
@@ -8802,9 +8318,7 @@
       </c>
     </row>
     <row r="241" spans="1:8">
-      <c r="A241" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A241" s="9"/>
       <c r="B241" s="6">
         <v>64145</v>
       </c>
@@ -8828,9 +8342,7 @@
       </c>
     </row>
     <row r="242" spans="1:8">
-      <c r="A242" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A242" s="9"/>
       <c r="B242" s="6">
         <v>64172</v>
       </c>
@@ -8854,9 +8366,7 @@
       </c>
     </row>
     <row r="243" spans="1:8">
-      <c r="A243" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A243" s="9"/>
       <c r="B243" s="6">
         <v>64237</v>
       </c>
@@ -8880,9 +8390,7 @@
       </c>
     </row>
     <row r="244" spans="1:8">
-      <c r="A244" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A244" s="9"/>
       <c r="B244" s="6">
         <v>64241</v>
       </c>
@@ -8906,9 +8414,7 @@
       </c>
     </row>
     <row r="245" spans="1:8">
-      <c r="A245" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A245" s="9"/>
       <c r="B245" s="6">
         <v>64189</v>
       </c>
@@ -8932,9 +8438,7 @@
       </c>
     </row>
     <row r="246" spans="1:8">
-      <c r="A246" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A246" s="9"/>
       <c r="B246" s="6">
         <v>64324</v>
       </c>
@@ -8958,9 +8462,7 @@
       </c>
     </row>
     <row r="247" spans="1:8">
-      <c r="A247" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A247" s="9"/>
       <c r="B247" s="6">
         <v>65161</v>
       </c>
@@ -8984,9 +8486,7 @@
       </c>
     </row>
     <row r="248" spans="1:8">
-      <c r="A248" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A248" s="9"/>
       <c r="B248" s="6">
         <v>65256</v>
       </c>
@@ -9010,9 +8510,7 @@
       </c>
     </row>
     <row r="249" spans="1:8">
-      <c r="A249" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A249" s="9"/>
       <c r="B249" s="6">
         <v>65542</v>
       </c>
@@ -9036,9 +8534,7 @@
       </c>
     </row>
     <row r="250" spans="1:8">
-      <c r="A250" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A250" s="9"/>
       <c r="B250" s="6">
         <v>65316</v>
       </c>
@@ -9062,9 +8558,7 @@
       </c>
     </row>
     <row r="251" spans="1:8">
-      <c r="A251" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A251" s="9"/>
       <c r="B251" s="6">
         <v>65583</v>
       </c>
@@ -9088,9 +8582,7 @@
       </c>
     </row>
     <row r="252" spans="1:8">
-      <c r="A252" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A252" s="9"/>
       <c r="B252" s="6">
         <v>65584</v>
       </c>
@@ -9114,9 +8606,7 @@
       </c>
     </row>
     <row r="253" spans="1:8">
-      <c r="A253" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A253" s="9"/>
       <c r="B253" s="6">
         <v>64165</v>
       </c>
@@ -9140,9 +8630,7 @@
       </c>
     </row>
     <row r="254" spans="1:8">
-      <c r="A254" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A254" s="9"/>
       <c r="B254" s="6">
         <v>64185</v>
       </c>
@@ -9166,9 +8654,7 @@
       </c>
     </row>
     <row r="255" spans="1:8">
-      <c r="A255" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A255" s="9"/>
       <c r="B255" s="6">
         <v>64276</v>
       </c>
@@ -9192,9 +8678,7 @@
       </c>
     </row>
     <row r="256" spans="1:8">
-      <c r="A256" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A256" s="9"/>
       <c r="B256" s="6">
         <v>64281</v>
       </c>
@@ -9218,9 +8702,7 @@
       </c>
     </row>
     <row r="257" spans="1:8">
-      <c r="A257" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A257" s="9"/>
       <c r="B257" s="6">
         <v>64286</v>
       </c>
@@ -9244,9 +8726,7 @@
       </c>
     </row>
     <row r="258" spans="1:8">
-      <c r="A258" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A258" s="9"/>
       <c r="B258" s="6">
         <v>64320</v>
       </c>
@@ -9270,9 +8750,7 @@
       </c>
     </row>
     <row r="259" spans="1:8">
-      <c r="A259" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A259" s="9"/>
       <c r="B259" s="6">
         <v>64477</v>
       </c>
@@ -9296,9 +8774,7 @@
       </c>
     </row>
     <row r="260" spans="1:8">
-      <c r="A260" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A260" s="9"/>
       <c r="B260" s="6">
         <v>65543</v>
       </c>
@@ -9320,9 +8796,7 @@
       </c>
     </row>
     <row r="261" spans="1:8">
-      <c r="A261" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A261" s="9"/>
       <c r="B261" s="6">
         <v>64473</v>
       </c>
@@ -9346,9 +8820,7 @@
       </c>
     </row>
     <row r="262" spans="1:8">
-      <c r="A262" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A262" s="9"/>
       <c r="B262" s="6">
         <v>64472</v>
       </c>
@@ -9372,9 +8844,7 @@
       </c>
     </row>
     <row r="263" spans="1:8">
-      <c r="A263" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A263" s="9"/>
       <c r="B263" s="6">
         <v>64167</v>
       </c>
@@ -9398,9 +8868,7 @@
       </c>
     </row>
     <row r="264" spans="1:8">
-      <c r="A264" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A264" s="9"/>
       <c r="B264" s="6">
         <v>64198</v>
       </c>
@@ -9424,9 +8892,7 @@
       </c>
     </row>
     <row r="265" spans="1:8">
-      <c r="A265" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A265" s="9"/>
       <c r="B265" s="6">
         <v>64266</v>
       </c>
@@ -9450,9 +8916,7 @@
       </c>
     </row>
     <row r="266" spans="1:8">
-      <c r="A266" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A266" s="9"/>
       <c r="B266" s="6">
         <v>64271</v>
       </c>
@@ -9476,9 +8940,7 @@
       </c>
     </row>
     <row r="267" spans="1:8">
-      <c r="A267" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A267" s="9"/>
       <c r="B267" s="6">
         <v>64316</v>
       </c>
@@ -9502,9 +8964,7 @@
       </c>
     </row>
     <row r="268" spans="1:8">
-      <c r="A268" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A268" s="9"/>
       <c r="B268" s="6">
         <v>64491</v>
       </c>
@@ -9528,9 +8988,7 @@
       </c>
     </row>
     <row r="269" spans="1:8">
-      <c r="A269" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A269" s="9"/>
       <c r="B269" s="6">
         <v>64809</v>
       </c>
@@ -9554,9 +9012,7 @@
       </c>
     </row>
     <row r="270" spans="1:8">
-      <c r="A270" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A270" s="9"/>
       <c r="B270" s="6">
         <v>64807</v>
       </c>
@@ -9580,9 +9036,7 @@
       </c>
     </row>
     <row r="271" spans="1:8">
-      <c r="A271" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A271" s="9"/>
       <c r="B271" s="6">
         <v>64492</v>
       </c>
@@ -9606,9 +9060,7 @@
       </c>
     </row>
     <row r="272" spans="1:8">
-      <c r="A272" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A272" s="9"/>
       <c r="B272" s="6">
         <v>64135</v>
       </c>
@@ -9632,9 +9084,7 @@
       </c>
     </row>
     <row r="273" spans="1:8">
-      <c r="A273" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A273" s="9"/>
       <c r="B273" s="6">
         <v>64139</v>
       </c>
@@ -9658,9 +9108,7 @@
       </c>
     </row>
     <row r="274" spans="1:8">
-      <c r="A274" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A274" s="9"/>
       <c r="B274" s="6">
         <v>64169</v>
       </c>
@@ -9684,9 +9132,7 @@
       </c>
     </row>
     <row r="275" spans="1:8">
-      <c r="A275" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A275" s="9"/>
       <c r="B275" s="6">
         <v>64200</v>
       </c>
@@ -9710,9 +9156,7 @@
       </c>
     </row>
     <row r="276" spans="1:8">
-      <c r="A276" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A276" s="9"/>
       <c r="B276" s="6">
         <v>64204</v>
       </c>
@@ -9736,9 +9180,7 @@
       </c>
     </row>
     <row r="277" spans="1:8">
-      <c r="A277" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A277" s="9"/>
       <c r="B277" s="6">
         <v>64208</v>
       </c>
@@ -9762,9 +9204,7 @@
       </c>
     </row>
     <row r="278" spans="1:8">
-      <c r="A278" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A278" s="9"/>
       <c r="B278" s="6">
         <v>64212</v>
       </c>
@@ -9788,9 +9228,7 @@
       </c>
     </row>
     <row r="279" spans="1:8">
-      <c r="A279" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A279" s="9"/>
       <c r="B279" s="6">
         <v>64216</v>
       </c>
@@ -9814,9 +9252,7 @@
       </c>
     </row>
     <row r="280" spans="1:8">
-      <c r="A280" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A280" s="9"/>
       <c r="B280" s="6">
         <v>64220</v>
       </c>
@@ -9840,9 +9276,7 @@
       </c>
     </row>
     <row r="281" spans="1:8">
-      <c r="A281" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A281" s="9"/>
       <c r="B281" s="6">
         <v>64225</v>
       </c>
@@ -9866,9 +9300,7 @@
       </c>
     </row>
     <row r="282" spans="1:8">
-      <c r="A282" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A282" s="9"/>
       <c r="B282" s="6">
         <v>64229</v>
       </c>
@@ -9892,9 +9324,7 @@
       </c>
     </row>
     <row r="283" spans="1:8">
-      <c r="A283" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A283" s="9"/>
       <c r="B283" s="6">
         <v>64234</v>
       </c>
@@ -9918,9 +9348,7 @@
       </c>
     </row>
     <row r="284" spans="1:8">
-      <c r="A284" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A284" s="9"/>
       <c r="B284" s="6">
         <v>64305</v>
       </c>
@@ -9944,9 +9372,7 @@
       </c>
     </row>
     <row r="285" spans="1:8">
-      <c r="A285" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A285" s="9"/>
       <c r="B285" s="6">
         <v>65550</v>
       </c>
@@ -9970,9 +9396,7 @@
       </c>
     </row>
     <row r="286" spans="1:8">
-      <c r="A286" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A286" s="9"/>
       <c r="B286" s="6">
         <v>65551</v>
       </c>
@@ -9996,9 +9420,7 @@
       </c>
     </row>
     <row r="287" spans="1:8">
-      <c r="A287" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A287" s="9"/>
       <c r="B287" s="6">
         <v>64327</v>
       </c>
@@ -10022,9 +9444,7 @@
       </c>
     </row>
     <row r="288" spans="1:8">
-      <c r="A288" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A288" s="9"/>
       <c r="B288" s="6">
         <v>64810</v>
       </c>
@@ -10048,9 +9468,7 @@
       </c>
     </row>
     <row r="289" spans="1:8">
-      <c r="A289" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A289" s="9"/>
       <c r="B289" s="6">
         <v>65244</v>
       </c>
@@ -10074,9 +9492,7 @@
       </c>
     </row>
     <row r="290" spans="1:8">
-      <c r="A290" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A290" s="9"/>
       <c r="B290" s="6">
         <v>65162</v>
       </c>
@@ -10100,9 +9516,7 @@
       </c>
     </row>
     <row r="291" spans="1:8">
-      <c r="A291" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A291" s="9"/>
       <c r="B291" s="6">
         <v>64278</v>
       </c>
@@ -10126,9 +9540,7 @@
       </c>
     </row>
     <row r="292" spans="1:8">
-      <c r="A292" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A292" s="9"/>
       <c r="B292" s="6">
         <v>64283</v>
       </c>
@@ -10152,9 +9564,7 @@
       </c>
     </row>
     <row r="293" spans="1:8">
-      <c r="A293" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A293" s="9"/>
       <c r="B293" s="6">
         <v>64288</v>
       </c>
@@ -10178,9 +9588,7 @@
       </c>
     </row>
     <row r="294" spans="1:8">
-      <c r="A294" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A294" s="9"/>
       <c r="B294" s="6">
         <v>64321</v>
       </c>
@@ -10204,9 +9612,7 @@
       </c>
     </row>
     <row r="295" spans="1:8">
-      <c r="A295" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A295" s="9"/>
       <c r="B295" s="6">
         <v>64819</v>
       </c>
@@ -10230,9 +9636,7 @@
       </c>
     </row>
     <row r="296" spans="1:8">
-      <c r="A296" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A296" s="9"/>
       <c r="B296" s="6">
         <v>65171</v>
       </c>
@@ -10256,9 +9660,7 @@
       </c>
     </row>
     <row r="297" spans="1:8">
-      <c r="A297" s="9">
-        <v>44988</v>
-      </c>
+      <c r="A297" s="9"/>
       <c r="B297" s="6">
         <v>65255</v>
       </c>

</xml_diff>